<commit_message>
Commiting Walton and Awardco excel files from an output file
</commit_message>
<xml_diff>
--- a/Integrations/4_AwardCo/AwardCo20221027181451310.xlsx
+++ b/Integrations/4_AwardCo/AwardCo20221027181451310.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Integrations\4_AwardCo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{522532EF-BF3E-467C-ACF4-79BD4052DF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C6D02FB-B36B-4705-96F8-D99A8AB0CCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930"/>
   </bookViews>
   <sheets>
     <sheet name="AwardCo20221027181451310" sheetId="1" r:id="rId1"/>
@@ -12919,7 +12919,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A1305" sqref="A1305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -70015,46 +70015,46 @@
       </c>
     </row>
     <row r="1305" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1305">
+      <c r="A1305" s="1">
         <v>159990</v>
       </c>
-      <c r="B1305" t="s">
+      <c r="B1305" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="C1305" t="s">
+      <c r="C1305" s="1" t="s">
         <v>3501</v>
       </c>
-      <c r="D1305" t="s">
+      <c r="D1305" s="1" t="s">
         <v>3502</v>
       </c>
-      <c r="E1305">
+      <c r="E1305" s="1">
         <v>159990</v>
       </c>
-      <c r="F1305" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1305">
+      <c r="F1305" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1305" s="1">
         <v>20220404</v>
       </c>
-      <c r="H1305">
+      <c r="H1305" s="1">
         <v>19770816</v>
       </c>
-      <c r="I1305">
+      <c r="I1305" s="1">
         <v>144361</v>
       </c>
-      <c r="J1305" t="s">
+      <c r="J1305" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K1305" t="s">
+      <c r="K1305" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1305" t="s">
+      <c r="L1305" s="1" t="s">
         <v>3503</v>
       </c>
-      <c r="M1305" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1305" t="s">
+      <c r="M1305" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1305" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>